<commit_message>
Task, Roles and Estimates Definition
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D433CD-666A-4008-A931-1E0F178599CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B46EF-50B9-4232-B74E-B5BE58F5DD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GANTT CHART" sheetId="8" r:id="rId1"/>
-    <sheet name="BURNDOWN CHART" sheetId="9" r:id="rId2"/>
+    <sheet name="TEAM" sheetId="10" r:id="rId1"/>
+    <sheet name="GANTT CHART" sheetId="8" r:id="rId2"/>
+    <sheet name="BURNDOWN CHART" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'GANTT CHART'!$A:$M</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'GANTT CHART'!$A:$M</definedName>
     <definedName name="color">'GANTT CHART'!$E1</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2017 Vertex42 LLC"</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
   <si>
     <t>TASK</t>
   </si>
@@ -112,9 +113,6 @@
     <t>Start Coding</t>
   </si>
   <si>
-    <t>2nd Delivery</t>
-  </si>
-  <si>
     <t>1st Delivery</t>
   </si>
   <si>
@@ -190,12 +188,6 @@
     <t>Tasks Assigned</t>
   </si>
   <si>
-    <t>Bernardo Carvalho: #X (Z hours) and #Y (W hours)</t>
-  </si>
-  <si>
-    <t>Estimate time for Bernardo should be Z+W hours</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -203,6 +195,60 @@
   </si>
   <si>
     <t>Ideal</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>João Félix (Product Owner)</t>
+  </si>
+  <si>
+    <t>Luís Lamy (Scrum Master)</t>
+  </si>
+  <si>
+    <t>Generate Sprint 1 Burndown Chart #3 (1 hour)</t>
+  </si>
+  <si>
+    <t>SysML diagram for 3 FR #4 (5 hours)</t>
+  </si>
+  <si>
+    <t>Model Main Business Process (BPMN) #5 (6 hours)</t>
+  </si>
+  <si>
+    <t>Implement Back-End Logic for Basic Features #8 (10 hours)</t>
+  </si>
+  <si>
+    <t>Design Front-End UI #6 (30 hours)</t>
+  </si>
+  <si>
+    <t>Implement Front-End #7 (7 hours)</t>
+  </si>
+  <si>
+    <t>Guilherme Santana (Quality Controller)</t>
+  </si>
+  <si>
+    <t>Gantt Chart and Task Dependencies #2 (3 hours)</t>
+  </si>
+  <si>
+    <t>Quality Check and Testing #9 (35 hours)</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Define Team Roles and Responsibilities #1 (0.5 hours)</t>
+  </si>
+  <si>
+    <t>Yaroslav Hayduk (Team Member)</t>
+  </si>
+  <si>
+    <t>Bernardo Carvalho (Team Member)</t>
+  </si>
+  <si>
+    <t>Working Days</t>
+  </si>
+  <si>
+    <t>Work divided by the whole team</t>
   </si>
 </sst>
 </file>
@@ -213,9 +259,9 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,8 +350,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,8 +404,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -533,21 +607,6 @@
       <left style="thin">
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
       <right/>
       <top style="thin">
         <color theme="4" tint="0.39994506668294322"/>
@@ -574,20 +633,22 @@
       <top style="thin">
         <color theme="4" tint="0.39994506668294322"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -599,7 +660,7 @@
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -710,6 +771,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -719,39 +786,99 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -2051,9 +2178,6 @@
               <c:f>'GANTT CHART'!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2nd Delivery</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2142,12 +2266,6 @@
               <c:numCache>
                 <c:formatCode>dd/mm/yy;@</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>45808</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45808</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2157,12 +2275,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2483,6 +2595,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BURNDOWN CHART'!$F$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>45755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45758</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45760</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45762</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45764</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45765</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45766</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45767</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45768</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45769</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45770</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45771</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45772</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45773</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'BURNDOWN CHART'!$F$14:$Y$14</c:f>
@@ -2490,64 +2671,64 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2577,6 +2758,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BURNDOWN CHART'!$F$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>45755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45758</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45759</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45760</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45761</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45762</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45763</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45764</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45765</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45766</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45767</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45768</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45769</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45770</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45771</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45772</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45773</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'BURNDOWN CHART'!$F$15:$Y$15</c:f>
@@ -2584,61 +2834,61 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>42.75</c:v>
+                  <c:v>208.52500000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.5</c:v>
+                  <c:v>197.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.25</c:v>
+                  <c:v>186.57499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>175.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.75</c:v>
+                  <c:v>164.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.5</c:v>
+                  <c:v>153.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.25</c:v>
+                  <c:v>142.67500000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>131.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.75</c:v>
+                  <c:v>120.72499999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.5</c:v>
+                  <c:v>109.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.25</c:v>
+                  <c:v>98.775000000000006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>87.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.75</c:v>
+                  <c:v>76.824999999999989</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.5</c:v>
+                  <c:v>65.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.25</c:v>
+                  <c:v>54.875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>43.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.75</c:v>
+                  <c:v>32.925000000000011</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5</c:v>
+                  <c:v>21.949999999999989</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.25</c:v>
+                  <c:v>10.974999999999994</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -3725,6 +3975,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF283FC5-4BF5-4EF5-8A21-CE5D1B5BCAD4}">
+  <dimension ref="B2:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B3" s="74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B4" s="74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" s="74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" s="74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3732,7 +4027,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:E14"/>
+      <selection activeCell="M6" sqref="M6:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3750,7 +4045,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -3818,6 +4113,9 @@
       </c>
       <c r="L4" s="13" t="s">
         <v>9</v>
+      </c>
+      <c r="M4" s="75" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -3835,11 +4133,11 @@
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="40" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="34">
         <v>45755</v>
@@ -3855,7 +4153,7 @@
         <v>45755</v>
       </c>
       <c r="G6" s="31">
-        <f t="shared" ref="G6:L14" si="0">IF(ISBLANK($D6),0,IF($E6=G$4,$D6-$C6+1,0))</f>
+        <f t="shared" ref="G6:M14" si="0">IF(ISBLANK($D6),0,IF($E6=G$4,$D6-$C6+1,0))</f>
         <v>1</v>
       </c>
       <c r="H6" s="31">
@@ -3878,11 +4176,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M6" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="34">
         <v>45755</v>
@@ -3921,13 +4222,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M7" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>35</v>
+      <c r="A8" s="40" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="34">
         <v>45756</v>
@@ -3966,11 +4270,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M8" s="32">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="34">
         <v>45757</v>
@@ -4009,11 +4316,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M9" s="32">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="34">
         <v>45759</v>
@@ -4052,13 +4362,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M10" s="32">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>29</v>
+      <c r="A11" s="37" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="34">
         <v>45762</v>
@@ -4097,13 +4410,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M11" s="32">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>28</v>
+      <c r="A12" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="34">
         <v>45763</v>
@@ -4142,11 +4458,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M12" s="32">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="34">
         <v>45765</v>
@@ -4185,13 +4504,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="M13" s="32">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>37</v>
+      <c r="A14" s="37" t="s">
+        <v>36</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="34">
         <v>45769</v>
@@ -4229,6 +4551,9 @@
       <c r="L14" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="M14" s="32">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
@@ -4246,6 +4571,10 @@
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="55"/>
     </row>
     <row r="19" spans="2:5" ht="22.8" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
@@ -4276,43 +4605,52 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="33">
+      <c r="B21" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="44">
         <v>45774</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="45">
         <v>0.25</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="45">
         <v>0.95</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="33">
-        <v>45808</v>
-      </c>
-      <c r="D22" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="24">
-        <v>0.95</v>
-      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="49"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
     </row>
     <row r="36" spans="1:1" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="E5:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$G$4:$L$4</formula1>
@@ -4325,12 +4663,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C6B9-B96F-4FA2-ABBE-ACB72B75F1F2}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4346,7 +4684,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -4417,1262 +4755,1433 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="62">
+        <v>45755</v>
+      </c>
+      <c r="G3" s="62">
+        <v>45756</v>
+      </c>
+      <c r="H3" s="62">
+        <v>45757</v>
+      </c>
+      <c r="I3" s="62">
+        <v>45758</v>
+      </c>
+      <c r="J3" s="62">
+        <v>45759</v>
+      </c>
+      <c r="K3" s="62">
+        <v>45760</v>
+      </c>
+      <c r="L3" s="62">
+        <v>45761</v>
+      </c>
+      <c r="M3" s="62">
+        <v>45762</v>
+      </c>
+      <c r="N3" s="62">
+        <v>45763</v>
+      </c>
+      <c r="O3" s="62">
+        <v>45764</v>
+      </c>
+      <c r="P3" s="62">
+        <v>45765</v>
+      </c>
+      <c r="Q3" s="62">
+        <v>45766</v>
+      </c>
+      <c r="R3" s="62">
+        <v>45767</v>
+      </c>
+      <c r="S3" s="62">
+        <v>45768</v>
+      </c>
+      <c r="T3" s="62">
+        <v>45769</v>
+      </c>
+      <c r="U3" s="62">
+        <v>45770</v>
+      </c>
+      <c r="V3" s="62">
+        <v>45771</v>
+      </c>
+      <c r="W3" s="62">
+        <v>45772</v>
+      </c>
+      <c r="X3" s="62">
+        <v>45773</v>
+      </c>
+      <c r="Y3" s="62">
+        <v>45774</v>
+      </c>
+      <c r="Z3" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="65">
+        <v>45755</v>
+      </c>
+      <c r="D4" s="56">
+        <v>45755</v>
+      </c>
+      <c r="E4" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="58">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57">
+        <f>E4-SUM(F4:Y4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="63"/>
+      <c r="B5" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="65">
+        <v>45755</v>
+      </c>
+      <c r="D5" s="56">
+        <v>45755</v>
+      </c>
+      <c r="E5" s="57">
+        <v>3</v>
+      </c>
+      <c r="F5" s="58">
+        <v>3</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="57">
+        <f t="shared" ref="Z5:Z12" si="0">E5-SUM(F5:Y5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="65">
+        <v>45756</v>
+      </c>
+      <c r="D6" s="56">
+        <v>45757</v>
+      </c>
+      <c r="E6" s="57">
+        <v>1</v>
+      </c>
+      <c r="F6" s="58">
+        <v>1</v>
+      </c>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
+      <c r="Y6" s="57"/>
+      <c r="Z6" s="57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="65">
+        <v>45757</v>
+      </c>
+      <c r="D7" s="56">
+        <v>45762</v>
+      </c>
+      <c r="E7" s="59">
+        <v>35</v>
+      </c>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="57"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
+      <c r="Y7" s="57"/>
+      <c r="Z7" s="57">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="65">
+        <v>45759</v>
+      </c>
+      <c r="D8" s="56">
+        <v>45763</v>
+      </c>
+      <c r="E8" s="59">
+        <v>30</v>
+      </c>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
+      <c r="Y8" s="57"/>
+      <c r="Z8" s="57">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="65">
+        <v>45762</v>
+      </c>
+      <c r="D9" s="56">
+        <v>45769</v>
+      </c>
+      <c r="E9" s="59">
+        <v>50</v>
+      </c>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="57"/>
+      <c r="V9" s="57"/>
+      <c r="W9" s="57"/>
+      <c r="X9" s="57"/>
+      <c r="Y9" s="57"/>
+      <c r="Z9" s="57">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="65">
+        <v>45763</v>
+      </c>
+      <c r="D10" s="56">
+        <v>45767</v>
+      </c>
+      <c r="E10" s="59">
+        <v>30</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="57"/>
+      <c r="X10" s="57"/>
+      <c r="Y10" s="57"/>
+      <c r="Z10" s="57">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="65">
+        <v>45765</v>
+      </c>
+      <c r="D11" s="56">
+        <v>45770</v>
+      </c>
+      <c r="E11" s="59">
+        <v>35</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="57"/>
+      <c r="Z11" s="57">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="65">
+        <v>45769</v>
+      </c>
+      <c r="D12" s="56">
+        <v>45774</v>
+      </c>
+      <c r="E12" s="59">
+        <v>35</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
+      <c r="Y12" s="57"/>
+      <c r="Z12" s="57">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D13" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="70">
+        <f>SUM(E4:E12)</f>
+        <v>219.5</v>
+      </c>
+      <c r="F13" s="70">
+        <f t="shared" ref="F13:Y13" si="1">SUM(F4:F12)</f>
+        <v>4.5</v>
+      </c>
+      <c r="G13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="70">
+        <f>SUM(Z4:Z12)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="77"/>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="70">
+        <f>E13</f>
+        <v>219.5</v>
+      </c>
+      <c r="F14" s="70">
+        <f>E14-F13</f>
+        <v>215</v>
+      </c>
+      <c r="G14" s="70">
+        <f t="shared" ref="G14:Y14" si="2">F14-G13</f>
+        <v>215</v>
+      </c>
+      <c r="H14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="I14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="J14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="K14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="L14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="M14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="N14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="O14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="P14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="Q14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="R14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="S14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="T14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="U14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="V14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="W14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="X14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="Y14" s="70">
+        <f t="shared" si="2"/>
+        <v>215</v>
+      </c>
+      <c r="Z14" s="39"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D15" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="57">
+        <f>E13</f>
+        <v>219.5</v>
+      </c>
+      <c r="F15" s="57">
+        <f>$E$15-F2*$E$15/COUNT($F$3:$Y$3)</f>
+        <v>208.52500000000001</v>
+      </c>
+      <c r="G15" s="57">
+        <f t="shared" ref="G15:Y15" si="3">$E$15-G2*$E$15/COUNT($F$3:$Y$3)</f>
+        <v>197.55</v>
+      </c>
+      <c r="H15" s="57">
+        <f t="shared" si="3"/>
+        <v>186.57499999999999</v>
+      </c>
+      <c r="I15" s="57">
+        <f t="shared" si="3"/>
+        <v>175.6</v>
+      </c>
+      <c r="J15" s="57">
+        <f t="shared" si="3"/>
+        <v>164.625</v>
+      </c>
+      <c r="K15" s="57">
+        <f t="shared" si="3"/>
+        <v>153.65</v>
+      </c>
+      <c r="L15" s="57">
+        <f t="shared" si="3"/>
+        <v>142.67500000000001</v>
+      </c>
+      <c r="M15" s="57">
+        <f t="shared" si="3"/>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="N15" s="57">
+        <f t="shared" si="3"/>
+        <v>120.72499999999999</v>
+      </c>
+      <c r="O15" s="57">
+        <f t="shared" si="3"/>
+        <v>109.75</v>
+      </c>
+      <c r="P15" s="57">
+        <f t="shared" si="3"/>
+        <v>98.775000000000006</v>
+      </c>
+      <c r="Q15" s="57">
+        <f t="shared" si="3"/>
+        <v>87.800000000000011</v>
+      </c>
+      <c r="R15" s="57">
+        <f t="shared" si="3"/>
+        <v>76.824999999999989</v>
+      </c>
+      <c r="S15" s="57">
+        <f t="shared" si="3"/>
+        <v>65.849999999999994</v>
+      </c>
+      <c r="T15" s="57">
+        <f t="shared" si="3"/>
+        <v>54.875</v>
+      </c>
+      <c r="U15" s="57">
+        <f t="shared" si="3"/>
+        <v>43.900000000000006</v>
+      </c>
+      <c r="V15" s="57">
+        <f t="shared" si="3"/>
+        <v>32.925000000000011</v>
+      </c>
+      <c r="W15" s="57">
+        <f t="shared" si="3"/>
+        <v>21.949999999999989</v>
+      </c>
+      <c r="X15" s="57">
+        <f t="shared" si="3"/>
+        <v>10.974999999999994</v>
+      </c>
+      <c r="Y15" s="57">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="39"/>
+    </row>
+    <row r="17" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="D17" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="41">
+      <c r="E17" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="62">
         <v>45755</v>
       </c>
-      <c r="G3" s="41">
+      <c r="G17" s="62">
         <v>45756</v>
       </c>
-      <c r="H3" s="41">
+      <c r="H17" s="62">
         <v>45757</v>
       </c>
-      <c r="I3" s="41">
+      <c r="I17" s="62">
         <v>45758</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J17" s="62">
         <v>45759</v>
       </c>
-      <c r="K3" s="41">
+      <c r="K17" s="62">
         <v>45760</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L17" s="62">
         <v>45761</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M17" s="62">
         <v>45762</v>
       </c>
-      <c r="N3" s="41">
+      <c r="N17" s="62">
         <v>45763</v>
       </c>
-      <c r="O3" s="41">
+      <c r="O17" s="62">
         <v>45764</v>
       </c>
-      <c r="P3" s="41">
+      <c r="P17" s="62">
         <v>45765</v>
       </c>
-      <c r="Q3" s="41">
+      <c r="Q17" s="62">
         <v>45766</v>
       </c>
-      <c r="R3" s="41">
+      <c r="R17" s="62">
         <v>45767</v>
       </c>
-      <c r="S3" s="41">
+      <c r="S17" s="62">
         <v>45768</v>
       </c>
-      <c r="T3" s="41">
+      <c r="T17" s="62">
         <v>45769</v>
       </c>
-      <c r="U3" s="41">
+      <c r="U17" s="62">
         <v>45770</v>
       </c>
-      <c r="V3" s="41">
+      <c r="V17" s="62">
         <v>45771</v>
       </c>
-      <c r="W3" s="41">
+      <c r="W17" s="62">
         <v>45772</v>
       </c>
-      <c r="X3" s="41">
+      <c r="X17" s="62">
         <v>45773</v>
       </c>
-      <c r="Y3" s="41">
+      <c r="Y17" s="62">
         <v>45774</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z17" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D18" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="57">
+        <v>30.1</v>
+      </c>
+      <c r="F18" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+      <c r="Y18" s="57"/>
+      <c r="Z18" s="57">
+        <f>E18-SUM(F18:Y18)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="73"/>
+      <c r="D19" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="57">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="F19" s="58">
+        <v>3.1</v>
+      </c>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57">
+        <f t="shared" ref="Z19:Z21" si="4">E19-SUM(F19:Y19)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="57">
+        <v>30.1</v>
+      </c>
+      <c r="F20" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D21" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="57">
+        <v>61.1</v>
+      </c>
+      <c r="F21" s="58">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="57"/>
+      <c r="R21" s="57"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
+      <c r="Y21" s="57"/>
+      <c r="Z21" s="57">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D22" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="57">
+        <v>30.1</v>
+      </c>
+      <c r="F22" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="57"/>
+      <c r="Z22" s="57">
+        <f>E22-SUM(F22:Y22)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D23" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="57">
+        <f>SUM(E18:E22)</f>
+        <v>219.49999999999997</v>
+      </c>
+      <c r="F23" s="57">
+        <f t="shared" ref="F23:Y23" si="5">SUM(F18:F22)</f>
+        <v>4.5</v>
+      </c>
+      <c r="G23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="57">
+        <f>SUM(Z18:Z22)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D24" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="57">
+        <f>E23</f>
+        <v>219.49999999999997</v>
+      </c>
+      <c r="F24" s="57">
+        <f>E24-F23</f>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="G24" s="57">
+        <f t="shared" ref="G24:Y24" si="6">F24-G23</f>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="H24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="I24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="J24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="K24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="L24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="M24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="N24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="O24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="P24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="Q24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="R24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="S24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="T24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="U24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="V24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="W24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="X24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="Y24" s="57">
+        <f t="shared" si="6"/>
+        <v>214.99999999999997</v>
+      </c>
+      <c r="Z24" s="38"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D25" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="57">
+        <f>E23</f>
+        <v>219.49999999999997</v>
+      </c>
+      <c r="F25" s="57">
+        <f>$E$25-F2*$E$25/COUNT($F$3:$Y$3)</f>
+        <v>208.52499999999998</v>
+      </c>
+      <c r="G25" s="57">
+        <f t="shared" ref="G25:Y25" si="7">$E$25-G2*$E$25/COUNT($F$3:$Y$3)</f>
+        <v>197.54999999999998</v>
+      </c>
+      <c r="H25" s="57">
+        <f t="shared" si="7"/>
+        <v>186.57499999999999</v>
+      </c>
+      <c r="I25" s="57">
+        <f t="shared" si="7"/>
+        <v>175.59999999999997</v>
+      </c>
+      <c r="J25" s="57">
+        <f t="shared" si="7"/>
+        <v>164.625</v>
+      </c>
+      <c r="K25" s="57">
+        <f t="shared" si="7"/>
+        <v>153.64999999999998</v>
+      </c>
+      <c r="L25" s="57">
+        <f t="shared" si="7"/>
+        <v>142.67499999999998</v>
+      </c>
+      <c r="M25" s="57">
+        <f t="shared" si="7"/>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="N25" s="57">
+        <f t="shared" si="7"/>
+        <v>120.72499999999998</v>
+      </c>
+      <c r="O25" s="57">
+        <f t="shared" si="7"/>
+        <v>109.75</v>
+      </c>
+      <c r="P25" s="57">
+        <f t="shared" si="7"/>
+        <v>98.774999999999991</v>
+      </c>
+      <c r="Q25" s="57">
+        <f t="shared" si="7"/>
+        <v>87.799999999999983</v>
+      </c>
+      <c r="R25" s="57">
+        <f t="shared" si="7"/>
+        <v>76.824999999999989</v>
+      </c>
+      <c r="S25" s="57">
+        <f t="shared" si="7"/>
+        <v>65.849999999999994</v>
+      </c>
+      <c r="T25" s="57">
+        <f t="shared" si="7"/>
+        <v>54.875</v>
+      </c>
+      <c r="U25" s="57">
+        <f t="shared" si="7"/>
+        <v>43.900000000000006</v>
+      </c>
+      <c r="V25" s="57">
+        <f t="shared" si="7"/>
+        <v>32.924999999999983</v>
+      </c>
+      <c r="W25" s="57">
+        <f t="shared" si="7"/>
+        <v>21.949999999999989</v>
+      </c>
+      <c r="X25" s="57">
+        <f t="shared" si="7"/>
+        <v>10.975000000000023</v>
+      </c>
+      <c r="Y25" s="57">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="38"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+    </row>
+    <row r="27" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="34">
-        <v>45755</v>
-      </c>
-      <c r="D4" s="35">
-        <v>45755</v>
-      </c>
-      <c r="E4" s="43">
-        <v>1</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="44">
-        <f>E4-SUM(F4:Y4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="34">
-        <v>45755</v>
-      </c>
-      <c r="D5" s="35">
-        <v>45755</v>
-      </c>
-      <c r="E5" s="43">
-        <v>2</v>
-      </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="44">
-        <f t="shared" ref="Z5:Z12" si="0">E5-SUM(F5:Y5)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="34">
-        <v>45756</v>
-      </c>
-      <c r="D6" s="35">
-        <v>45757</v>
-      </c>
-      <c r="E6" s="43">
-        <v>3</v>
-      </c>
-      <c r="F6" s="43">
-        <v>1</v>
-      </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="44">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="34">
-        <v>45757</v>
-      </c>
-      <c r="D7" s="35">
-        <v>45762</v>
-      </c>
-      <c r="E7" s="43">
-        <v>4</v>
-      </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="44">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="34">
-        <v>45759</v>
-      </c>
-      <c r="D8" s="35">
-        <v>45763</v>
-      </c>
-      <c r="E8" s="43">
-        <v>5</v>
-      </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="34">
-        <v>45762</v>
-      </c>
-      <c r="D9" s="35">
-        <v>45769</v>
-      </c>
-      <c r="E9" s="43">
-        <v>6</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43"/>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="44">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="34">
-        <v>45763</v>
-      </c>
-      <c r="D10" s="35">
-        <v>45767</v>
-      </c>
-      <c r="E10" s="43">
-        <v>7</v>
-      </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="44">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="34">
-        <v>45765</v>
-      </c>
-      <c r="D11" s="35">
-        <v>45770</v>
-      </c>
-      <c r="E11" s="43">
-        <v>8</v>
-      </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="44">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="34">
-        <v>45769</v>
-      </c>
-      <c r="D12" s="35">
-        <v>45774</v>
-      </c>
-      <c r="E12" s="43">
-        <v>9</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="44">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D13" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="49">
-        <f>SUM(E4:E12)</f>
-        <v>45</v>
-      </c>
-      <c r="F13" s="49">
-        <f t="shared" ref="F13:Y13" si="1">SUM(F4:F12)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="49">
-        <f>SUM(Z4:Z12)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D14" s="47" t="s">
+    <row r="29" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A29" s="74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A32" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="49">
-        <f>E13</f>
-        <v>45</v>
-      </c>
-      <c r="F14" s="49">
-        <f>E14-F13</f>
-        <v>44</v>
-      </c>
-      <c r="G14" s="49">
-        <f t="shared" ref="G14:Y14" si="2">F14-G13</f>
-        <v>44</v>
-      </c>
-      <c r="H14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="I14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="J14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="K14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="L14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="M14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="N14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="O14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="P14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="Q14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="R14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="S14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="T14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="U14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="V14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="W14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="X14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="Y14" s="49">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-      <c r="Z14" s="49"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D15" s="47" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A38" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="51">
-        <f>E13</f>
-        <v>45</v>
-      </c>
-      <c r="F15" s="51">
-        <f>$E$15-F2*$E$15/COUNT($F$3:$Y$3)</f>
-        <v>42.75</v>
-      </c>
-      <c r="G15" s="51">
-        <f t="shared" ref="G15:Y15" si="3">$E$15-G2*$E$15/COUNT($F$3:$Y$3)</f>
-        <v>40.5</v>
-      </c>
-      <c r="H15" s="51">
-        <f t="shared" si="3"/>
-        <v>38.25</v>
-      </c>
-      <c r="I15" s="51">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="J15" s="51">
-        <f t="shared" si="3"/>
-        <v>33.75</v>
-      </c>
-      <c r="K15" s="51">
-        <f t="shared" si="3"/>
-        <v>31.5</v>
-      </c>
-      <c r="L15" s="51">
-        <f t="shared" si="3"/>
-        <v>29.25</v>
-      </c>
-      <c r="M15" s="51">
-        <f t="shared" si="3"/>
-        <v>27</v>
-      </c>
-      <c r="N15" s="51">
-        <f t="shared" si="3"/>
-        <v>24.75</v>
-      </c>
-      <c r="O15" s="51">
-        <f t="shared" si="3"/>
-        <v>22.5</v>
-      </c>
-      <c r="P15" s="51">
-        <f t="shared" si="3"/>
-        <v>20.25</v>
-      </c>
-      <c r="Q15" s="51">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="R15" s="51">
-        <f t="shared" si="3"/>
-        <v>15.75</v>
-      </c>
-      <c r="S15" s="51">
-        <f t="shared" si="3"/>
-        <v>13.5</v>
-      </c>
-      <c r="T15" s="51">
-        <f t="shared" si="3"/>
-        <v>11.25</v>
-      </c>
-      <c r="U15" s="51">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="V15" s="51">
-        <f t="shared" si="3"/>
-        <v>6.75</v>
-      </c>
-      <c r="W15" s="51">
-        <f t="shared" si="3"/>
-        <v>4.5</v>
-      </c>
-      <c r="X15" s="51">
-        <f t="shared" si="3"/>
-        <v>2.25</v>
-      </c>
-      <c r="Y15" s="51">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="49"/>
-    </row>
-    <row r="17" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="41">
-        <v>45755</v>
-      </c>
-      <c r="G17" s="41">
-        <v>45756</v>
-      </c>
-      <c r="H17" s="41">
-        <v>45757</v>
-      </c>
-      <c r="I17" s="41">
-        <v>45758</v>
-      </c>
-      <c r="J17" s="41">
-        <v>45759</v>
-      </c>
-      <c r="K17" s="41">
-        <v>45760</v>
-      </c>
-      <c r="L17" s="41">
-        <v>45761</v>
-      </c>
-      <c r="M17" s="41">
-        <v>45762</v>
-      </c>
-      <c r="N17" s="41">
-        <v>45763</v>
-      </c>
-      <c r="O17" s="41">
-        <v>45764</v>
-      </c>
-      <c r="P17" s="41">
-        <v>45765</v>
-      </c>
-      <c r="Q17" s="41">
-        <v>45766</v>
-      </c>
-      <c r="R17" s="41">
-        <v>45767</v>
-      </c>
-      <c r="S17" s="41">
-        <v>45768</v>
-      </c>
-      <c r="T17" s="41">
-        <v>45769</v>
-      </c>
-      <c r="U17" s="41">
-        <v>45770</v>
-      </c>
-      <c r="V17" s="41">
-        <v>45771</v>
-      </c>
-      <c r="W17" s="41">
-        <v>45772</v>
-      </c>
-      <c r="X17" s="41">
-        <v>45773</v>
-      </c>
-      <c r="Y17" s="41">
-        <v>45774</v>
-      </c>
-      <c r="Z17" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="43">
-        <v>9</v>
-      </c>
-      <c r="F18" s="43">
-        <v>1</v>
-      </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="44">
-        <f>E18-SUM(F18:Y18)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="43">
-        <v>9</v>
-      </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
-      <c r="U19" s="43"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="43"/>
-      <c r="X19" s="43"/>
-      <c r="Y19" s="43"/>
-      <c r="Z19" s="44">
-        <f t="shared" ref="Z19:Z21" si="4">E19-SUM(F19:Y19)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="43">
-        <v>9</v>
-      </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43">
-        <v>1</v>
-      </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="44">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D21" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="43">
-        <v>9</v>
-      </c>
-      <c r="F21" s="43">
-        <v>1</v>
-      </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="43"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="44">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D22" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="43">
-        <v>9</v>
-      </c>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45"/>
-      <c r="X22" s="45"/>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="44">
-        <f>E22-SUM(F22:Y22)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D23" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="50">
-        <f>SUM(E18:E22)</f>
-        <v>45</v>
-      </c>
-      <c r="F23" s="50">
-        <f t="shared" ref="F23:Y23" si="5">SUM(F18:F22)</f>
-        <v>2</v>
-      </c>
-      <c r="G23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="50">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y23" s="50">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="50">
-        <f>SUM(Z18:Z22)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D24" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="51">
-        <f>E23</f>
-        <v>45</v>
-      </c>
-      <c r="F24" s="51">
-        <f>E24-F23</f>
-        <v>43</v>
-      </c>
-      <c r="G24" s="51">
-        <f t="shared" ref="G24:Y24" si="6">F24-G23</f>
-        <v>43</v>
-      </c>
-      <c r="H24" s="51">
-        <f t="shared" si="6"/>
-        <v>43</v>
-      </c>
-      <c r="I24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="J24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="K24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="L24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="M24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="N24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="O24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="P24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="Q24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="R24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="S24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="T24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="U24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="V24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="W24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="X24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="Y24" s="51">
-        <f t="shared" si="6"/>
-        <v>42</v>
-      </c>
-      <c r="Z24" s="42"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D25" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="51">
-        <f>E23</f>
-        <v>45</v>
-      </c>
-      <c r="F25" s="51">
-        <f>$E$25-F2*$E$25/COUNT($F$3:$Y$3)</f>
-        <v>42.75</v>
-      </c>
-      <c r="G25" s="51">
-        <f t="shared" ref="G25:Y25" si="7">$E$25-G2*$E$25/COUNT($F$3:$Y$3)</f>
-        <v>40.5</v>
-      </c>
-      <c r="H25" s="51">
-        <f t="shared" si="7"/>
-        <v>38.25</v>
-      </c>
-      <c r="I25" s="51">
-        <f t="shared" si="7"/>
-        <v>36</v>
-      </c>
-      <c r="J25" s="51">
-        <f t="shared" si="7"/>
-        <v>33.75</v>
-      </c>
-      <c r="K25" s="51">
-        <f t="shared" si="7"/>
-        <v>31.5</v>
-      </c>
-      <c r="L25" s="51">
-        <f t="shared" si="7"/>
-        <v>29.25</v>
-      </c>
-      <c r="M25" s="51">
-        <f t="shared" si="7"/>
-        <v>27</v>
-      </c>
-      <c r="N25" s="51">
-        <f t="shared" si="7"/>
-        <v>24.75</v>
-      </c>
-      <c r="O25" s="51">
-        <f t="shared" si="7"/>
-        <v>22.5</v>
-      </c>
-      <c r="P25" s="51">
-        <f t="shared" si="7"/>
-        <v>20.25</v>
-      </c>
-      <c r="Q25" s="51">
-        <f t="shared" si="7"/>
-        <v>18</v>
-      </c>
-      <c r="R25" s="51">
-        <f t="shared" si="7"/>
-        <v>15.75</v>
-      </c>
-      <c r="S25" s="51">
-        <f t="shared" si="7"/>
-        <v>13.5</v>
-      </c>
-      <c r="T25" s="51">
-        <f t="shared" si="7"/>
-        <v>11.25</v>
-      </c>
-      <c r="U25" s="51">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="V25" s="51">
-        <f t="shared" si="7"/>
-        <v>6.75</v>
-      </c>
-      <c r="W25" s="51">
-        <f t="shared" si="7"/>
-        <v>4.5</v>
-      </c>
-      <c r="X25" s="51">
-        <f t="shared" si="7"/>
-        <v>2.25</v>
-      </c>
-      <c r="Y25" s="51">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="42"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="42"/>
-      <c r="W26" s="42"/>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="42"/>
-      <c r="Z26" s="42"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A46" s="74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="54"/>
+    </row>
+    <row r="55" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A55" s="74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A61" s="74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5681,7 +6190,7 @@
     <mergeCell ref="A10:A11"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D18:D22 E4:Z12 E25 E18:Z24 E15:Y15 F25:Z26" xr:uid="{71679858-1939-4B9F-A4D7-63892D4A7839}">
+    <dataValidation type="list" allowBlank="1" sqref="D18:D22 F25:Z26 E25 E4:E6 E15:Y15 F4:Z12 E18:Z24" xr:uid="{71679858-1939-4B9F-A4D7-63892D4A7839}">
       <formula1>$G$3:$L$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
BPMNs and Update Hours
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisl\OneDrive\Documentos\GitHub\msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A2A072-C409-42BC-B6B1-89D905DECB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A45EEB-B667-43E1-8312-2124C38A699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2691,34 +2691,34 @@
                   <c:v>193.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>193.75</c:v>
+                  <c:v>192.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4645,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C6B9-B96F-4FA2-ABBE-ACB72B75F1F2}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5018,7 +5018,9 @@
       <c r="O8" s="65">
         <v>2</v>
       </c>
-      <c r="P8" s="66"/>
+      <c r="P8" s="65">
+        <v>1</v>
+      </c>
       <c r="Q8" s="66"/>
       <c r="R8" s="66"/>
       <c r="S8" s="66"/>
@@ -5030,7 +5032,7 @@
       <c r="Y8" s="66"/>
       <c r="Z8" s="66">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -5247,7 +5249,7 @@
       </c>
       <c r="P13" s="68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13" s="68">
         <f t="shared" si="1"/>
@@ -5287,7 +5289,7 @@
       </c>
       <c r="Z13" s="68">
         <f>SUM(Z4:Z12)</f>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -5344,43 +5346,43 @@
       </c>
       <c r="P14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="Q14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="R14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="S14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="T14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="U14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="V14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="W14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="X14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="Y14" s="68">
         <f t="shared" si="2"/>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
       <c r="Z14" s="39"/>
     </row>
@@ -5681,7 +5683,9 @@
       <c r="O21" s="65">
         <v>2</v>
       </c>
-      <c r="P21" s="66"/>
+      <c r="P21" s="65">
+        <v>1</v>
+      </c>
       <c r="Q21" s="66"/>
       <c r="R21" s="66"/>
       <c r="S21" s="66"/>
@@ -5693,7 +5697,7 @@
       <c r="Y21" s="66"/>
       <c r="Z21" s="66">
         <f t="shared" si="4"/>
-        <v>56.75</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -5788,7 +5792,7 @@
       </c>
       <c r="P23" s="66">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="66">
         <f t="shared" si="5"/>
@@ -5828,7 +5832,7 @@
       </c>
       <c r="Z23" s="66">
         <f>SUM(Z18:Z22)</f>
-        <v>193.75</v>
+        <v>192.75</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -5881,43 +5885,43 @@
       </c>
       <c r="P24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="Q24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="R24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="S24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="T24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="U24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="V24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="W24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="X24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="Y24" s="66">
         <f t="shared" si="6"/>
-        <v>193.74999999999997</v>
+        <v>192.74999999999997</v>
       </c>
       <c r="Z24" s="38"/>
     </row>

</xml_diff>

<commit_message>
#5 #12 #13 BPMN's Done
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfel\OneDrive\Desktop\MSP-24-25\msp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guipi\Documents\eu\SST_FCT_UNL_MIEI\5Ano\MSP\msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA7E188-C46F-4582-BCD0-44C99DF5FFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6DE6C5-C1C9-46BE-A320-B30DD2BE8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEAM" sheetId="10" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="BURNDOWN CHART" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'GANTT CHART'!$A:$M</definedName>
     <definedName name="color">'GANTT CHART'!$E1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'GANTT CHART'!$A:$M</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2017 Vertex42 LLC"</definedName>
     <definedName name="vertex42_id" hidden="1">"project-timeline.xlsx"</definedName>
@@ -861,27 +861,27 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1010,7 +1010,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2508,7 +2508,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2707,31 +2707,31 @@
                   <c:v>187.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>187.75</c:v>
+                  <c:v>187.25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>187.75</c:v>
+                  <c:v>185.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3985,34 +3985,34 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="61" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
         <v>63</v>
       </c>
@@ -4033,20 +4033,20 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="47.69921875" customWidth="1"/>
-    <col min="3" max="3" width="9.69921875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="47.75" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="6.8984375" customWidth="1"/>
+    <col min="7" max="7" width="6.875" customWidth="1"/>
     <col min="8" max="13" width="6" customWidth="1"/>
     <col min="15" max="15" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -4080,7 +4080,7 @@
       <c r="K3" s="28"/>
       <c r="L3" s="29"/>
     </row>
-    <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
@@ -4135,8 +4135,8 @@
       <c r="K5" s="7"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="72" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -4183,8 +4183,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="73"/>
       <c r="B7" s="21" t="s">
         <v>25</v>
       </c>
@@ -4229,8 +4229,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="70" t="s">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="72" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -4277,8 +4277,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="74"/>
       <c r="B9" s="21" t="s">
         <v>24</v>
       </c>
@@ -4323,8 +4323,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="73"/>
       <c r="B10" s="21" t="s">
         <v>66</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>27</v>
       </c>
@@ -4417,8 +4417,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+    <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="72" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -4465,8 +4465,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
+    <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
       <c r="B13" s="21" t="s">
         <v>29</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>35</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16" t="s">
@@ -4576,10 +4576,10 @@
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="49"/>
     </row>
-    <row r="19" spans="2:5" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="24" x14ac:dyDescent="0.2">
       <c r="B19" s="9" t="s">
         <v>14</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>20</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="40" t="s">
         <v>21</v>
       </c>
@@ -4621,19 +4621,19 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="45"/>
       <c r="C22" s="46"/>
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="43"/>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
     </row>
-    <row r="36" spans="1:1" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A36" s="1"/>
     </row>
   </sheetData>
@@ -4658,22 +4658,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C6B9-B96F-4FA2-ABBE-ACB72B75F1F2}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.8984375" customWidth="1"/>
-    <col min="2" max="2" width="48.8984375" customWidth="1"/>
-    <col min="3" max="3" width="17.296875" customWidth="1"/>
-    <col min="4" max="4" width="17.8984375" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="6" max="25" width="8.69921875" customWidth="1"/>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="2" max="2" width="48.875" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="25" width="8.75" customWidth="1"/>
     <col min="26" max="26" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -4682,7 +4682,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
       <c r="F2">
         <v>1</v>
@@ -4745,7 +4745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
         <v>13</v>
       </c>
@@ -4825,8 +4825,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="75" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="63" t="s">
@@ -4868,8 +4868,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="75"/>
       <c r="B5" s="63" t="s">
         <v>25</v>
       </c>
@@ -4909,8 +4909,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="73" t="s">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="75" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="63" t="s">
@@ -4952,8 +4952,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="75"/>
       <c r="B7" s="57" t="s">
         <v>24</v>
       </c>
@@ -4986,7 +4986,7 @@
       <c r="O7" s="65">
         <v>1.5</v>
       </c>
-      <c r="P7" s="75">
+      <c r="P7" s="71">
         <v>4</v>
       </c>
       <c r="Q7" s="66"/>
@@ -5003,8 +5003,8 @@
         <v>18.25</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="75"/>
       <c r="B8" s="57" t="s">
         <v>66</v>
       </c>
@@ -5036,8 +5036,12 @@
       <c r="P8" s="65">
         <v>1</v>
       </c>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
+      <c r="Q8" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="R8" s="71">
+        <v>2</v>
+      </c>
       <c r="S8" s="66"/>
       <c r="T8" s="66"/>
       <c r="U8" s="66"/>
@@ -5047,10 +5051,10 @@
       <c r="Y8" s="66"/>
       <c r="Z8" s="66">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="54" t="s">
         <v>27</v>
       </c>
@@ -5091,8 +5095,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="75" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="55" t="s">
@@ -5134,8 +5138,8 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="73"/>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="75"/>
       <c r="B11" s="57" t="s">
         <v>29</v>
       </c>
@@ -5173,7 +5177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>35</v>
       </c>
@@ -5214,7 +5218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D13" s="58" t="s">
         <v>45</v>
       </c>
@@ -5268,11 +5272,11 @@
       </c>
       <c r="Q13" s="68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R13" s="68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S13" s="68">
         <f t="shared" si="1"/>
@@ -5304,10 +5308,10 @@
       </c>
       <c r="Z13" s="68">
         <f>SUM(Z4:Z12)</f>
-        <v>187.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>185.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="64"/>
       <c r="B14" t="s">
         <v>65</v>
@@ -5365,43 +5369,43 @@
       </c>
       <c r="Q14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>187.25</v>
       </c>
       <c r="R14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="S14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="T14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="U14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="V14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="W14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="X14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="Y14" s="68">
         <f t="shared" si="2"/>
-        <v>187.75</v>
+        <v>185.25</v>
       </c>
       <c r="Z14" s="39"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D15" s="58" t="s">
         <v>47</v>
       </c>
@@ -5491,7 +5495,7 @@
       </c>
       <c r="Z15" s="39"/>
     </row>
-    <row r="17" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="D17" s="52" t="s">
         <v>37</v>
@@ -5563,7 +5567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D18" s="59" t="s">
         <v>38</v>
       </c>
@@ -5601,7 +5605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D19" s="59" t="s">
         <v>39</v>
       </c>
@@ -5621,8 +5625,12 @@
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
       <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="66"/>
+      <c r="Q19" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="R19" s="71">
+        <v>2</v>
+      </c>
       <c r="S19" s="66"/>
       <c r="T19" s="66"/>
       <c r="U19" s="66"/>
@@ -5632,10 +5640,10 @@
       <c r="Y19" s="66"/>
       <c r="Z19" s="66">
         <f t="shared" ref="Z19:Z21" si="4">E19-SUM(F19:Y19)</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+        <v>62.499999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D20" s="59" t="s">
         <v>40</v>
       </c>
@@ -5656,11 +5664,11 @@
       <c r="M20" s="65">
         <v>2</v>
       </c>
-      <c r="N20" s="75">
+      <c r="N20" s="71">
         <v>1</v>
       </c>
       <c r="O20" s="66"/>
-      <c r="P20" s="75">
+      <c r="P20" s="71">
         <v>4</v>
       </c>
       <c r="Q20" s="66"/>
@@ -5677,7 +5685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D21" s="59" t="s">
         <v>41</v>
       </c>
@@ -5719,7 +5727,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D22" s="59" t="s">
         <v>42</v>
       </c>
@@ -5761,7 +5769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D23" s="60" t="s">
         <v>45</v>
       </c>
@@ -5815,11 +5823,11 @@
       </c>
       <c r="Q23" s="66">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R23" s="66">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S23" s="66">
         <f t="shared" si="5"/>
@@ -5851,10 +5859,10 @@
       </c>
       <c r="Z23" s="66">
         <f>SUM(Z18:Z22)</f>
-        <v>187.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+        <v>185.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D24" s="60" t="s">
         <v>46</v>
       </c>
@@ -5908,43 +5916,43 @@
       </c>
       <c r="Q24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>187.24999999999997</v>
       </c>
       <c r="R24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="S24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="T24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="U24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="V24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="W24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="X24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="Y24" s="66">
         <f t="shared" si="6"/>
-        <v>187.74999999999997</v>
+        <v>185.24999999999997</v>
       </c>
       <c r="Z24" s="38"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D25" s="60" t="s">
         <v>47</v>
       </c>
@@ -6034,7 +6042,7 @@
       </c>
       <c r="Z25" s="38"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
@@ -6057,177 +6065,178 @@
       <c r="Y26" s="38"/>
       <c r="Z26" s="38"/>
     </row>
-    <row r="27" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="67" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="67"/>
     </row>
-    <row r="32" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="61" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="74" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="74"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="74" t="s">
+      <c r="B33" s="70"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="74"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="70"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="67" t="s">
         <v>51</v>
       </c>
       <c r="B39" s="67"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="64" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="64"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="s">
         <v>53</v>
       </c>
       <c r="B41" s="64"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="64" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="64"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="67" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="67"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="64" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="64"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E53" s="48"/>
     </row>
-    <row r="54" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="64"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="64" t="s">
         <v>53</v>
       </c>
       <c r="B56" s="64"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="61" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="64" t="s">
         <v>52</v>
       </c>
       <c r="B61" s="64"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="64" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="64"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
#4 #11 #14 #15 SysMl completed
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guipi\Documents\eu\SST_FCT_UNL_MIEI\5Ano\MSP\msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6DE6C5-C1C9-46BE-A320-B30DD2BE8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFAA03-E139-4815-BAE9-FDAFA94D5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2713,25 +2713,25 @@
                   <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4658,8 +4658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C6B9-B96F-4FA2-ABBE-ACB72B75F1F2}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4991,7 +4991,9 @@
       </c>
       <c r="Q7" s="66"/>
       <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
+      <c r="S7" s="71">
+        <v>5.5</v>
+      </c>
       <c r="T7" s="66"/>
       <c r="U7" s="66"/>
       <c r="V7" s="66"/>
@@ -5000,7 +5002,7 @@
       <c r="Y7" s="66"/>
       <c r="Z7" s="66">
         <f t="shared" si="0"/>
-        <v>18.25</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -5280,7 +5282,7 @@
       </c>
       <c r="S13" s="68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="T13" s="68">
         <f t="shared" si="1"/>
@@ -5308,7 +5310,7 @@
       </c>
       <c r="Z13" s="68">
         <f>SUM(Z4:Z12)</f>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -5377,31 +5379,31 @@
       </c>
       <c r="S14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="T14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="U14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="V14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="W14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="X14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="Y14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="Z14" s="39"/>
     </row>
@@ -5631,7 +5633,9 @@
       <c r="R19" s="71">
         <v>2</v>
       </c>
-      <c r="S19" s="66"/>
+      <c r="S19" s="71">
+        <v>5.5</v>
+      </c>
       <c r="T19" s="66"/>
       <c r="U19" s="66"/>
       <c r="V19" s="66"/>
@@ -5640,7 +5644,7 @@
       <c r="Y19" s="66"/>
       <c r="Z19" s="66">
         <f t="shared" ref="Z19:Z21" si="4">E19-SUM(F19:Y19)</f>
-        <v>62.499999999999993</v>
+        <v>56.999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -5831,7 +5835,7 @@
       </c>
       <c r="S23" s="66">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="T23" s="66">
         <f t="shared" si="5"/>
@@ -5859,7 +5863,7 @@
       </c>
       <c r="Z23" s="66">
         <f>SUM(Z18:Z22)</f>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -5924,31 +5928,31 @@
       </c>
       <c r="S24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="T24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="U24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="V24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="W24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="X24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="Y24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="Z24" s="38"/>
     </row>

</xml_diff>

<commit_message>
#5 #10 #12 #13 SysMl completed
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guipi\Documents\eu\SST_FCT_UNL_MIEI\5Ano\MSP\msp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6DE6C5-C1C9-46BE-A320-B30DD2BE8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFAA03-E139-4815-BAE9-FDAFA94D5535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2713,25 +2713,25 @@
                   <c:v>185.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>185.25</c:v>
+                  <c:v>179.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4658,8 +4658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3C6B9-B96F-4FA2-ABBE-ACB72B75F1F2}">
   <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4991,7 +4991,9 @@
       </c>
       <c r="Q7" s="66"/>
       <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
+      <c r="S7" s="71">
+        <v>5.5</v>
+      </c>
       <c r="T7" s="66"/>
       <c r="U7" s="66"/>
       <c r="V7" s="66"/>
@@ -5000,7 +5002,7 @@
       <c r="Y7" s="66"/>
       <c r="Z7" s="66">
         <f t="shared" si="0"/>
-        <v>18.25</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -5280,7 +5282,7 @@
       </c>
       <c r="S13" s="68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="T13" s="68">
         <f t="shared" si="1"/>
@@ -5308,7 +5310,7 @@
       </c>
       <c r="Z13" s="68">
         <f>SUM(Z4:Z12)</f>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -5377,31 +5379,31 @@
       </c>
       <c r="S14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="T14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="U14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="V14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="W14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="X14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="Y14" s="68">
         <f t="shared" si="2"/>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
       <c r="Z14" s="39"/>
     </row>
@@ -5631,7 +5633,9 @@
       <c r="R19" s="71">
         <v>2</v>
       </c>
-      <c r="S19" s="66"/>
+      <c r="S19" s="71">
+        <v>5.5</v>
+      </c>
       <c r="T19" s="66"/>
       <c r="U19" s="66"/>
       <c r="V19" s="66"/>
@@ -5640,7 +5644,7 @@
       <c r="Y19" s="66"/>
       <c r="Z19" s="66">
         <f t="shared" ref="Z19:Z21" si="4">E19-SUM(F19:Y19)</f>
-        <v>62.499999999999993</v>
+        <v>56.999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -5831,7 +5835,7 @@
       </c>
       <c r="S23" s="66">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="T23" s="66">
         <f t="shared" si="5"/>
@@ -5859,7 +5863,7 @@
       </c>
       <c r="Z23" s="66">
         <f>SUM(Z18:Z22)</f>
-        <v>185.25</v>
+        <v>179.75</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -5924,31 +5928,31 @@
       </c>
       <c r="S24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="T24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="U24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="V24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="W24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="X24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="Y24" s="66">
         <f t="shared" si="6"/>
-        <v>185.24999999999997</v>
+        <v>179.74999999999997</v>
       </c>
       <c r="Z24" s="38"/>
     </row>

</xml_diff>